<commit_message>
BCBanHang: sửa lại file template (bỏ dòng Tổng cộng)
</commit_message>
<xml_diff>
--- a/banhang24/Template/ExportExcel/Report/BaoCaoBanHang/Teamplate_BaoCaoBanHangChiTietTheoKhachHang.xlsx
+++ b/banhang24/Template/ExportExcel/Report/BaoCaoBanHang/Teamplate_BaoCaoBanHangChiTietTheoKhachHang.xlsx
@@ -17,10 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <t>Tổng cộng:</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Mã hàng</t>
   </si>
@@ -114,7 +111,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -126,14 +123,8 @@
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="5">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -159,30 +150,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -194,7 +161,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -209,7 +176,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -228,26 +194,14 @@
     <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -554,111 +508,111 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O29"/>
+  <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomLeft" activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" style="8" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" style="7" customWidth="1"/>
     <col min="2" max="2" width="34.28515625" style="4" customWidth="1"/>
     <col min="3" max="3" width="21.28515625" style="4" customWidth="1"/>
     <col min="4" max="4" width="20.7109375" style="4" customWidth="1"/>
-    <col min="5" max="8" width="20.7109375" style="11" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" style="11" customWidth="1"/>
-    <col min="10" max="11" width="19.7109375" style="11" customWidth="1"/>
-    <col min="12" max="12" width="18" style="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18" style="11" customWidth="1"/>
-    <col min="14" max="14" width="14.7109375" style="11" customWidth="1"/>
+    <col min="5" max="8" width="20.7109375" style="10" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" style="10" customWidth="1"/>
+    <col min="10" max="11" width="19.7109375" style="10" customWidth="1"/>
+    <col min="12" max="12" width="18" style="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18" style="10" customWidth="1"/>
+    <col min="14" max="14" width="14.7109375" style="10" customWidth="1"/>
     <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="2"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="8"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+    </row>
+    <row r="4" spans="1:15" s="5" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="M4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="2"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="17"/>
-    </row>
-    <row r="4" spans="1:15" s="5" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="10" t="s">
+      <c r="N4" s="9" t="s">
         <v>5</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="I4" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="K4" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="L4" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="M4" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="N4" s="10" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -666,439 +620,390 @@
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="12"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="12"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="12"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="12"/>
-      <c r="N12" s="12"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="12"/>
-      <c r="N13" s="12"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12"/>
-      <c r="N14" s="12"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="12"/>
-      <c r="M15" s="12"/>
-      <c r="N15" s="12"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="11"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="12"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="11"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="12"/>
-      <c r="N17" s="12"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="11"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="12"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="12"/>
-      <c r="M18" s="12"/>
-      <c r="N18" s="12"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="11"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
-      <c r="K19" s="12"/>
-      <c r="L19" s="12"/>
-      <c r="M19" s="12"/>
-      <c r="N19" s="12"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
+      <c r="N19" s="11"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="12"/>
-      <c r="K20" s="12"/>
-      <c r="L20" s="12"/>
-      <c r="M20" s="12"/>
-      <c r="N20" s="12"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="11"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
-      <c r="K21" s="12"/>
-      <c r="L21" s="12"/>
-      <c r="M21" s="12"/>
-      <c r="N21" s="12"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="11"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="12"/>
-      <c r="K22" s="12"/>
-      <c r="L22" s="12"/>
-      <c r="M22" s="12"/>
-      <c r="N22" s="12"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="11"/>
+      <c r="N22" s="11"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="12"/>
-      <c r="K23" s="12"/>
-      <c r="L23" s="12"/>
-      <c r="M23" s="12"/>
-      <c r="N23" s="12"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="11"/>
+      <c r="L23" s="11"/>
+      <c r="M23" s="11"/>
+      <c r="N23" s="11"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="12"/>
-      <c r="J24" s="12"/>
-      <c r="K24" s="12"/>
-      <c r="L24" s="12"/>
-      <c r="M24" s="12"/>
-      <c r="N24" s="12"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="11"/>
+      <c r="N24" s="11"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="12"/>
-      <c r="J25" s="12"/>
-      <c r="K25" s="12"/>
-      <c r="L25" s="12"/>
-      <c r="M25" s="12"/>
-      <c r="N25" s="12"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11"/>
+      <c r="M25" s="11"/>
+      <c r="N25" s="11"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="12"/>
-      <c r="J26" s="12"/>
-      <c r="K26" s="12"/>
-      <c r="L26" s="12"/>
-      <c r="M26" s="12"/>
-      <c r="N26" s="12"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="11"/>
+      <c r="M26" s="11"/>
+      <c r="N26" s="11"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="12"/>
-      <c r="J27" s="12"/>
-      <c r="K27" s="12"/>
-      <c r="L27" s="12"/>
-      <c r="M27" s="12"/>
-      <c r="N27" s="12"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="11"/>
+      <c r="L27" s="11"/>
+      <c r="M27" s="11"/>
+      <c r="N27" s="11"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
-      <c r="I28" s="12"/>
-      <c r="J28" s="12"/>
-      <c r="K28" s="12"/>
-      <c r="L28" s="12"/>
-      <c r="M28" s="12"/>
-      <c r="N28" s="12"/>
-    </row>
-    <row r="29" spans="1:14" s="6" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="B29" s="18"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="13">
-        <f>SUM(E$5:E28)</f>
-        <v>0</v>
-      </c>
-      <c r="F29" s="13">
-        <f>SUM(F$5:F28)</f>
-        <v>0</v>
-      </c>
-      <c r="G29" s="13">
-        <f>SUM(G$5:G28)</f>
-        <v>0</v>
-      </c>
-      <c r="H29" s="13">
-        <f>SUM(H$5:H28)</f>
-        <v>0</v>
-      </c>
-      <c r="I29" s="14">
-        <f>SUM(I$5:I28)</f>
-        <v>0</v>
-      </c>
-      <c r="J29" s="14">
-        <f>SUM(J$5:J28)</f>
-        <v>0</v>
-      </c>
-      <c r="K29" s="14">
-        <f>SUM(K$5:K28)</f>
-        <v>0</v>
-      </c>
-      <c r="L29" s="14">
-        <f>SUM(L$5:L28)</f>
-        <v>0</v>
-      </c>
-      <c r="M29" s="14">
-        <f>SUM(M$5:M28)</f>
-        <v>0</v>
-      </c>
-      <c r="N29" s="14">
-        <f>SUM(N$5:N28)</f>
-        <v>0</v>
-      </c>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="11"/>
+      <c r="L28" s="11"/>
+      <c r="M28" s="11"/>
+      <c r="N28" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="A1:N1"/>
     <mergeCell ref="A2:N2"/>
     <mergeCell ref="L3:N3"/>
-    <mergeCell ref="A29:D29"/>
   </mergeCells>
   <pageMargins left="0.76" right="0.23" top="0.78" bottom="0.87" header="0.3" footer="0.7"/>
   <pageSetup scale="95" orientation="landscape" r:id="rId1"/>

</xml_diff>